<commit_message>
T8A - com gráfico de resíduos e análise estatística
</commit_message>
<xml_diff>
--- a/T8A - Condensadores.xlsx
+++ b/T8A - Condensadores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive - Universidade do Porto\Ambiente de Trabalho\GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C98C93-7382-450B-9310-526667402A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128AFF1B-8ACB-40BA-8832-1192EF29E82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <r>
       <t>R (</t>
@@ -137,11 +137,77 @@
       <t>(s)</t>
     </r>
   </si>
+  <si>
+    <t>Análise estatísitca</t>
+  </si>
+  <si>
+    <t>Declive (m)</t>
+  </si>
+  <si>
+    <t>u(m)</t>
+  </si>
+  <si>
+    <t>Ordenada na origem (b)</t>
+  </si>
+  <si>
+    <t>u(b)</t>
+  </si>
+  <si>
+    <t>t1/2=mR</t>
+  </si>
+  <si>
+    <t>t1/2=0,693RC</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>C=t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1/2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / (R*0,693)</t>
+    </r>
+  </si>
+  <si>
+    <t>Valor de C do declive:</t>
+  </si>
+  <si>
+    <t>C = declive / 0,693</t>
+  </si>
+  <si>
+    <t>Valor de C do multímetro:</t>
+  </si>
+  <si>
+    <t>Erro percentual:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,15 +231,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -196,13 +268,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -223,7 +344,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -254,15 +375,15 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t>t</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="-25000"/>
+              <a:rPr lang="en-US" sz="1600" baseline="-25000"/>
               <a:t>1/2</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="1600" baseline="0"/>
               <a:t>(R)</a:t>
             </a:r>
           </a:p>
@@ -293,13 +414,23 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15112538421033297"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.81217390594449412"/>
+          <c:h val="0.58880431612715078"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -307,15 +438,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Folha1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>t1/2(s)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>t1/2(R)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -339,6 +462,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.42000649024626197"/>
+                  <c:y val="-6.0010571595217263E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Folha1!$A$2:$A$20</c:f>
@@ -473,15 +646,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pt-PT"/>
+                  <a:rPr lang="pt-PT" sz="1400"/>
                   <a:t>R(</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="el-GR"/>
+                  <a:rPr lang="el-GR" sz="1400"/>
                   <a:t>Ω</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pt-PT"/>
+                  <a:rPr lang="pt-PT" sz="1400"/>
                   <a:t>)</a:t>
                 </a:r>
               </a:p>
@@ -512,7 +685,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -550,11 +723,11 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="353967568"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-2.0000000000000008E-5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -598,15 +771,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pt-PT"/>
+                  <a:rPr lang="pt-PT" sz="1400"/>
                   <a:t>t</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pt-PT" baseline="-25000"/>
+                  <a:rPr lang="pt-PT" sz="1400" baseline="-25000"/>
                   <a:t>1/2</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="pt-PT"/>
+                  <a:rPr lang="pt-PT" sz="1400"/>
                   <a:t>(S)</a:t>
                 </a:r>
               </a:p>
@@ -637,7 +810,445 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pt-PT"/>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="353970480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.70586673361008712"/>
+          <c:y val="0.58716389617964426"/>
+          <c:w val="0.24225048268655375"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600"/>
+              <a:t>Resíduos</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18530096237970253"/>
+          <c:y val="0.18300925925925926"/>
+          <c:w val="0.77903237095363076"/>
+          <c:h val="0.58880431612715078"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Resíduos</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$E$2:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F47D-4B2E-A8BA-754B688B73ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="459903503"/>
+        <c:axId val="459904751"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="459903503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>R(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Ω</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="800">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -675,10 +1286,144 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353970480"/>
+        <c:crossAx val="459904751"/>
+        <c:crossesAt val="-1.0000000000000004E-5"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="459904751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>t</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400" b="0" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>1/2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>(S)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="800">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="459903503"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -696,15 +1441,17 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.71256496062992114"/>
-          <c:y val="0.71577500729075527"/>
-          <c:w val="0.11243503937007876"/>
+          <c:x val="0.82343985126859143"/>
+          <c:y val="0.67512685914260728"/>
+          <c:w val="0.13489348206474192"/>
           <c:h val="7.8125546806649182E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
           <a:solidFill>
             <a:schemeClr val="tx1"/>
@@ -729,7 +1476,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -766,7 +1513,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -817,7 +1564,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1366,6 +2669,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEC8B28E-B863-4B96-9829-E69391AEC2FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1637,227 +2976,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="1">
-        <f>B2*0.000001</f>
+        <f t="shared" ref="C2:C6" si="0">B2*0.000001</f>
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1" t="e">
+        <f>A2*$I$20+$J$20</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E2" s="1" t="e">
+        <f>D2-C2</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C19" si="0">B3*0.000001</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="1" t="e">
+        <f t="shared" ref="D3:D20" si="1">A3*$I$20+$J$20</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E3" s="1" t="e">
+        <f t="shared" ref="E3:E20" si="2">D3-C3</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E4" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E5" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E6" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C7:C19" si="3">B7*0.000001</f>
         <v>0</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E7" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E8" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E9" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E10" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E11" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E12" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E13" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E15" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E16" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E17" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1">
         <f>B20*0.000001</f>
         <v>0</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E20" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="4" t="e">
+        <f t="array" ref="I20:J21">LINEST(C2:C20,A2:A20,TRUE,TRUE)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J20" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="H21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="J21" s="4" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" t="e">
+        <f>I20/0.693</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="12" t="e">
+        <f>ABS(D43-D44)/D44</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="C41:D41"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
T8A - com dados da aula
</commit_message>
<xml_diff>
--- a/T8A - Condensadores.xlsx
+++ b/T8A - Condensadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128AFF1B-8ACB-40BA-8832-1192EF29E82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A505A4A-C3CF-4EF7-835F-A32750DF6E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -298,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -311,19 +311,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,13 +517,51 @@
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Folha1!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Valor de C do declive:</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Valor de C do multímetro:</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Erro percentual:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -528,61 +570,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.1999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>9.9999999999999991E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.1999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.5999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.9999999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.9999999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.1999999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1.9999999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1068,75 +1083,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Folha1!$A$2:$A$20</c:f>
+              <c:f>Folha1!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$E$2:$E$20</c:f>
+              <c:f>Folha1!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-2.6181818181818207E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.5636363636363612E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.7454545454545435E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>-7.2727272727274002E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-1.8909090909090915E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.9090909090909059E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4.7272727272727288E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4.6545454545454548E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>-3.1636363636363622E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>-9.8181818181818006E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2976,10 +2994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2988,6 +3006,7 @@
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
     <col min="8" max="8" width="11.21875" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
@@ -3011,344 +3030,276 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="9"/>
+      <c r="A2" s="1">
+        <v>100</v>
+      </c>
+      <c r="B2" s="6">
+        <v>120</v>
+      </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:C6" si="0">B2*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="e">
+        <v>1.1999999999999999E-4</v>
+      </c>
+      <c r="D2" s="1">
         <f>A2*$I$20+$J$20</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E2" s="1" t="e">
+        <v>9.3818181818181782E-5</v>
+      </c>
+      <c r="E2" s="1">
         <f>D2-C2</f>
-        <v>#VALUE!</v>
+        <v>-2.6181818181818207E-5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="1">
+        <v>200</v>
+      </c>
+      <c r="B3" s="7">
+        <v>100</v>
+      </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="e">
+        <v>9.9999999999999991E-5</v>
+      </c>
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D20" si="1">A3*$I$20+$J$20</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E3" s="1" t="e">
+        <v>1.156363636363636E-4</v>
+      </c>
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E20" si="2">D3-C3</f>
-        <v>#VALUE!</v>
+        <v>1.5636363636363612E-5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="1">
+        <v>300</v>
+      </c>
+      <c r="B4" s="7">
+        <v>120</v>
+      </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="e">
+        <v>1.1999999999999999E-4</v>
+      </c>
+      <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E4" s="1" t="e">
+        <v>1.3745454545454542E-4</v>
+      </c>
+      <c r="E4" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>1.7454545454545435E-5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="1">
+        <v>400</v>
+      </c>
+      <c r="B5" s="7">
+        <v>160</v>
+      </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="e">
+        <v>1.5999999999999999E-4</v>
+      </c>
+      <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E5" s="1" t="e">
+        <v>1.5927272727272725E-4</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>-7.2727272727274002E-7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="1">
+        <v>500</v>
+      </c>
+      <c r="B6" s="8">
+        <v>200</v>
+      </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="e">
+        <v>1.9999999999999998E-4</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E6" s="1" t="e">
+        <v>1.8109090909090907E-4</v>
+      </c>
+      <c r="E6" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>-1.8909090909090915E-5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="1">
+        <v>600</v>
+      </c>
+      <c r="B7" s="7">
+        <v>200</v>
+      </c>
       <c r="C7" s="1">
         <f t="shared" ref="C7:C19" si="3">B7*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="e">
+        <v>1.9999999999999998E-4</v>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E7" s="1" t="e">
+        <v>2.0290909090909089E-4</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>2.9090909090909059E-6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="1">
+        <v>700</v>
+      </c>
+      <c r="B8" s="8">
+        <v>220</v>
+      </c>
       <c r="C8" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="e">
+        <v>2.1999999999999998E-4</v>
+      </c>
+      <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E8" s="1" t="e">
+        <v>2.2472727272727271E-4</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>4.7272727272727288E-6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="1">
+        <v>800</v>
+      </c>
+      <c r="B9" s="8">
+        <v>200</v>
+      </c>
       <c r="C9" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="e">
+        <v>1.9999999999999998E-4</v>
+      </c>
+      <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E9" s="1" t="e">
+        <v>2.4654545454545453E-4</v>
+      </c>
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>4.6545454545454548E-5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1">
+        <v>900</v>
+      </c>
+      <c r="B10" s="1">
+        <v>300</v>
+      </c>
       <c r="C10" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="e">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E10" s="1" t="e">
+        <v>2.6836363636363635E-4</v>
+      </c>
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>-3.1636363636363622E-5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>300</v>
+      </c>
       <c r="C11" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="e">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E11" s="1" t="e">
+        <v>2.9018181818181817E-4</v>
+      </c>
+      <c r="E11" s="1">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E12" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E13" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E14" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>-9.8181818181818006E-6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E15" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="A15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="1">
+        <f>I20/0.693</f>
+        <v>3.1483667847304217E-7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E16" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="A16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="12">
+        <v>3.4999999999999998E-7</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E17" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E18" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="A17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="13">
+        <f>ABS(D15-D16)/D16</f>
+        <v>0.10046663293416519</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="6"/>
+      <c r="J19" s="10"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1">
-        <f>B20*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E20" s="1" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="H20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="4" t="e">
-        <f t="array" ref="I20:J21">LINEST(C2:C20,A2:A20,TRUE,TRUE)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="J20" s="4" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K20" s="7" t="s">
+      <c r="I20" s="4">
+        <f t="array" ref="I20:J21">LINEST(C2:C11,A2:A11,TRUE,TRUE)</f>
+        <v>2.1818181818181821E-7</v>
+      </c>
+      <c r="J20" s="4">
+        <v>7.1999999999999961E-5</v>
+      </c>
+      <c r="K20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="4" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="J21" s="4" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="I21" s="4">
+        <v>2.7212053721992292E-8</v>
+      </c>
+      <c r="J21" s="4">
+        <v>1.6884635296354758E-5</v>
+      </c>
+      <c r="K21" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="10"/>
     </row>
     <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -3357,10 +3308,10 @@
       <c r="B40" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
@@ -3369,47 +3320,21 @@
       <c r="B41" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="8"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" t="e">
-        <f>I20/0.693</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="8"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="12" t="e">
-        <f>ABS(D43-D44)/D44</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="D41" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B43:C43"/>
     <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
T8A - com coisas que o ariel disse no feedback
</commit_message>
<xml_diff>
--- a/T8A - Condensadores.xlsx
+++ b/T8A - Condensadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00CB701-60FF-4BA8-87B2-DC2F979D2CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685AF77E-A947-469D-BE6A-13B27610D9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <r>
       <t>R (</t>
@@ -202,6 +202,18 @@
   <si>
     <t>Valor USB</t>
   </si>
+  <si>
+    <t>fit + sy</t>
+  </si>
+  <si>
+    <t>fit - sy</t>
+  </si>
+  <si>
+    <t>sy</t>
+  </si>
+  <si>
+    <t>r^2</t>
+  </si>
 </sst>
 </file>
 
@@ -301,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -320,27 +332,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -352,6 +349,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,12 +565,41 @@
           <c:errBars>
             <c:errDir val="x"/>
             <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="1"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Folha1!$N$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>0.1</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Folha1!$N$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>0.1</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:noFill/>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
                 <a:round/>
               </a:ln>
               <a:effectLst/>
@@ -557,8 +608,32 @@
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Folha1!$O$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>9.9999999999999995E-8</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Folha1!$O$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>9.9999999999999995E-8</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -655,6 +730,264 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5ACA-470A-B9D9-A27B39E6FD11}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>+sy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="6350" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>217.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>317.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>417.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>517.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>617.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>717.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>817.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>917.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1017.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1117.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$N$2:$N$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.1853475704431481E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4035293886249664E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6217112068067844E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8398930249886029E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0580748431704208E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.276256661352239E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4944384795340575E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7126202977158752E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9308021158976934E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1489839340795116E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9A5A-4F52-BD39-B54C87E77BBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>-sy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="6350" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>217.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>317.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>417.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>517.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>617.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>717.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>817.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>917.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1017.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1117.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$O$2:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.9101606592048836E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0919788410230657E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1273797022841246E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3455615204659431E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5637433386477611E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7819251568295793E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0001069750113975E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2182887931932154E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4364706113750336E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.6546524295568519E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9A5A-4F52-BD39-B54C87E77BBD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -938,14 +1271,30 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.70586673361008712"/>
-          <c:y val="0.58716389617964426"/>
-          <c:w val="0.24225048268655375"/>
-          <c:h val="0.15625109361329836"/>
+          <c:x val="0.69860060520863909"/>
+          <c:y val="0.57377320094561257"/>
+          <c:w val="0.21904952072869155"/>
+          <c:h val="0.16835304340977023"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1179,37 +1528,37 @@
             <c:numRef>
               <c:f>Folha1!$E$2:$E$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-2.6181818181818166E-5</c:v>
+                  <c:v>2.6181818181818166E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5636363636363653E-5</c:v>
+                  <c:v>-1.5636363636363653E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7454545454545462E-5</c:v>
+                  <c:v>-1.7454545454545462E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.2727272727268581E-7</c:v>
+                  <c:v>7.2727272727268581E-7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.8909090909090888E-5</c:v>
+                  <c:v>1.8909090909090888E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.909090909090933E-6</c:v>
+                  <c:v>-2.909090909090933E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.7272727272727559E-6</c:v>
+                  <c:v>-4.7272727272727559E-6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.6545454545454548E-5</c:v>
+                  <c:v>-4.6545454545454548E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-3.1636363636363622E-5</c:v>
+                  <c:v>3.1636363636363622E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-9.8181818181818006E-6</c:v>
+                  <c:v>9.8181818181818006E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,7 +1712,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="459904751"/>
-        <c:crossesAt val="-1.0000000000000004E-5"/>
+        <c:crossesAt val="-10000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -2749,13 +3098,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>606335</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>2474</xdr:rowOff>
+      <xdr:rowOff>177734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>94706</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>43544</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>35924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3046,15 +3395,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.5546875" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" customWidth="1"/>
@@ -3065,24 +3415,30 @@
     <col min="15" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <f>100+117.2</f>
         <v>217.2</v>
@@ -3090,20 +3446,28 @@
       <c r="B2" s="4">
         <v>120</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="10">
         <f t="shared" ref="C2:C6" si="0">B2*0.000001</f>
         <v>1.1999999999999999E-4</v>
       </c>
-      <c r="D2" s="13">
-        <f>A2*$D$20+$E$20</f>
+      <c r="D2" s="10">
+        <f t="shared" ref="D2:D11" si="1">A2*$D$20+$E$20</f>
         <v>9.3818181818181823E-5</v>
       </c>
-      <c r="E2" s="1">
-        <f>D2-C2</f>
-        <v>-2.6181818181818166E-5</v>
+      <c r="E2" s="10">
+        <f>C2-D2</f>
+        <v>2.6181818181818166E-5</v>
+      </c>
+      <c r="N2" s="25">
+        <f>D2+$E$22</f>
+        <v>1.1853475704431481E-4</v>
+      </c>
+      <c r="O2" s="25">
+        <f>D2-$E$22</f>
+        <v>6.9101606592048836E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>200+117.2</f>
         <v>317.2</v>
@@ -3111,20 +3475,28 @@
       <c r="B3" s="5">
         <v>100</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <f t="shared" si="0"/>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="D3" s="13">
-        <f>A3*$D$20+$E$20</f>
+      <c r="D3" s="10">
+        <f t="shared" si="1"/>
         <v>1.1563636363636364E-4</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E11" si="1">D3-C3</f>
-        <v>1.5636363636363653E-5</v>
+      <c r="E3" s="10">
+        <f t="shared" ref="E3:E11" si="2">C3-D3</f>
+        <v>-1.5636363636363653E-5</v>
+      </c>
+      <c r="N3" s="25">
+        <f t="shared" ref="N3:N11" si="3">D3+$E$22</f>
+        <v>1.4035293886249664E-4</v>
+      </c>
+      <c r="O3" s="25">
+        <f t="shared" ref="O3:O11" si="4">D3-$E$22</f>
+        <v>9.0919788410230657E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>300+117.2</f>
         <v>417.2</v>
@@ -3132,20 +3504,28 @@
       <c r="B4" s="5">
         <v>120</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="10">
         <f t="shared" si="0"/>
         <v>1.1999999999999999E-4</v>
       </c>
-      <c r="D4" s="13">
-        <f>A4*$D$20+$E$20</f>
+      <c r="D4" s="10">
+        <f t="shared" si="1"/>
         <v>1.3745454545454545E-4</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7454545454545462E-5</v>
+      <c r="E4" s="10">
+        <f t="shared" si="2"/>
+        <v>-1.7454545454545462E-5</v>
+      </c>
+      <c r="N4" s="25">
+        <f t="shared" si="3"/>
+        <v>1.6217112068067844E-4</v>
+      </c>
+      <c r="O4" s="25">
+        <f t="shared" si="4"/>
+        <v>1.1273797022841246E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f>400+117.2</f>
         <v>517.20000000000005</v>
@@ -3153,20 +3533,28 @@
       <c r="B5" s="5">
         <v>160</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="10">
         <f t="shared" si="0"/>
         <v>1.5999999999999999E-4</v>
       </c>
-      <c r="D5" s="13">
-        <f>A5*$D$20+$E$20</f>
+      <c r="D5" s="10">
+        <f t="shared" si="1"/>
         <v>1.592727272727273E-4</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" si="1"/>
-        <v>-7.2727272727268581E-7</v>
+      <c r="E5" s="10">
+        <f t="shared" si="2"/>
+        <v>7.2727272727268581E-7</v>
+      </c>
+      <c r="N5" s="25">
+        <f t="shared" si="3"/>
+        <v>1.8398930249886029E-4</v>
+      </c>
+      <c r="O5" s="25">
+        <f t="shared" si="4"/>
+        <v>1.3455615204659431E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f>500+117.2</f>
         <v>617.20000000000005</v>
@@ -3174,20 +3562,28 @@
       <c r="B6" s="6">
         <v>200</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="10">
         <f t="shared" si="0"/>
         <v>1.9999999999999998E-4</v>
       </c>
-      <c r="D6" s="13">
-        <f>A6*$D$20+$E$20</f>
+      <c r="D6" s="10">
+        <f t="shared" si="1"/>
         <v>1.8109090909090909E-4</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.8909090909090888E-5</v>
+      <c r="E6" s="10">
+        <f t="shared" si="2"/>
+        <v>1.8909090909090888E-5</v>
+      </c>
+      <c r="N6" s="25">
+        <f t="shared" si="3"/>
+        <v>2.0580748431704208E-4</v>
+      </c>
+      <c r="O6" s="25">
+        <f t="shared" si="4"/>
+        <v>1.5637433386477611E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f>600+117.2</f>
         <v>717.2</v>
@@ -3195,20 +3591,28 @@
       <c r="B7" s="5">
         <v>200</v>
       </c>
-      <c r="C7" s="13">
-        <f t="shared" ref="C7:C11" si="2">B7*0.000001</f>
+      <c r="C7" s="10">
+        <f t="shared" ref="C7:C11" si="5">B7*0.000001</f>
         <v>1.9999999999999998E-4</v>
       </c>
-      <c r="D7" s="13">
-        <f>A7*$D$20+$E$20</f>
+      <c r="D7" s="10">
+        <f t="shared" si="1"/>
         <v>2.0290909090909092E-4</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" si="1"/>
-        <v>2.909090909090933E-6</v>
+      <c r="E7" s="10">
+        <f t="shared" si="2"/>
+        <v>-2.909090909090933E-6</v>
+      </c>
+      <c r="N7" s="25">
+        <f t="shared" si="3"/>
+        <v>2.276256661352239E-4</v>
+      </c>
+      <c r="O7" s="25">
+        <f t="shared" si="4"/>
+        <v>1.7819251568295793E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>700+117.2</f>
         <v>817.2</v>
@@ -3216,20 +3620,28 @@
       <c r="B8" s="6">
         <v>220</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
+        <f t="shared" si="5"/>
+        <v>2.1999999999999998E-4</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="1"/>
+        <v>2.2472727272727274E-4</v>
+      </c>
+      <c r="E8" s="10">
         <f t="shared" si="2"/>
-        <v>2.1999999999999998E-4</v>
-      </c>
-      <c r="D8" s="13">
-        <f>A8*$D$20+$E$20</f>
-        <v>2.2472727272727274E-4</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="1"/>
-        <v>4.7272727272727559E-6</v>
+        <v>-4.7272727272727559E-6</v>
+      </c>
+      <c r="N8" s="25">
+        <f t="shared" si="3"/>
+        <v>2.4944384795340575E-4</v>
+      </c>
+      <c r="O8" s="25">
+        <f t="shared" si="4"/>
+        <v>2.0001069750113975E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f>800+117.2</f>
         <v>917.2</v>
@@ -3237,20 +3649,28 @@
       <c r="B9" s="6">
         <v>200</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="10">
+        <f t="shared" si="5"/>
+        <v>1.9999999999999998E-4</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="1"/>
+        <v>2.4654545454545453E-4</v>
+      </c>
+      <c r="E9" s="10">
         <f t="shared" si="2"/>
-        <v>1.9999999999999998E-4</v>
-      </c>
-      <c r="D9" s="13">
-        <f>A9*$D$20+$E$20</f>
-        <v>2.4654545454545453E-4</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>4.6545454545454548E-5</v>
+        <v>-4.6545454545454548E-5</v>
+      </c>
+      <c r="N9" s="25">
+        <f t="shared" si="3"/>
+        <v>2.7126202977158752E-4</v>
+      </c>
+      <c r="O9" s="25">
+        <f t="shared" si="4"/>
+        <v>2.2182887931932154E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f>900+117.2</f>
         <v>1017.2</v>
@@ -3258,20 +3678,28 @@
       <c r="B10" s="1">
         <v>300</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="10">
+        <f t="shared" si="5"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>2.6836363636363635E-4</v>
+      </c>
+      <c r="E10" s="10">
         <f t="shared" si="2"/>
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="D10" s="13">
-        <f>A10*$D$20+$E$20</f>
-        <v>2.6836363636363635E-4</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.1636363636363622E-5</v>
+        <v>3.1636363636363622E-5</v>
+      </c>
+      <c r="N10" s="25">
+        <f t="shared" si="3"/>
+        <v>2.9308021158976934E-4</v>
+      </c>
+      <c r="O10" s="25">
+        <f t="shared" si="4"/>
+        <v>2.4364706113750336E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f>1000+117.2</f>
         <v>1117.2</v>
@@ -3279,81 +3707,97 @@
       <c r="B11" s="1">
         <v>300</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="10">
+        <f t="shared" si="5"/>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="1"/>
+        <v>2.9018181818181817E-4</v>
+      </c>
+      <c r="E11" s="10">
         <f t="shared" si="2"/>
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="D11" s="13">
-        <f>A11*$D$20+$E$20</f>
-        <v>2.9018181818181817E-4</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="1"/>
-        <v>-9.8181818181818006E-6</v>
+        <v>9.8181818181818006E-6</v>
+      </c>
+      <c r="N11" s="25">
+        <f t="shared" si="3"/>
+        <v>3.1489839340795116E-4</v>
+      </c>
+      <c r="O11" s="25">
+        <f t="shared" si="4"/>
+        <v>2.6546524295568519E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>0.1</v>
+      </c>
+      <c r="O13" s="25">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="10">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="19">
         <f>D20/0.693</f>
         <v>3.1483667847304207E-7</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="12">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="20">
         <v>3.4999999999999998E-7</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="11">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="21">
         <f>ABS(D15-D16)/D16</f>
         <v>0.10046663293416548</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="3">
-        <f t="array" ref="D20:E21">LINEST(C2:C11,A2:A11,TRUE,TRUE)</f>
+        <f t="array" ref="D20:E22">LINEST(C2:C11,A2:A11,TRUE,TRUE)</f>
         <v>2.1818181818181815E-7</v>
       </c>
       <c r="E20" s="3">
         <v>4.6429090909090923E-5</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="17"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="3">
@@ -3365,65 +3809,80 @@
       <c r="F21" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="17"/>
+      <c r="G21" s="18"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="C23" s="17" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C22" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.88932806324110669</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2.4716575226132987E-5</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="24"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="7"/>
+      <c r="C24" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="15" t="s">
+      <c r="D24" s="18"/>
+      <c r="E24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15" t="s">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="19" t="s">
+      <c r="H24" s="17"/>
+      <c r="I24" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B24" s="20" t="s">
+    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="B25" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C25" s="19">
         <v>233</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10">
+      <c r="D25" s="19"/>
+      <c r="E25" s="19">
         <v>226</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="11">
-        <f>ABS(C24-E24)/E24</f>
+      <c r="F25" s="19"/>
+      <c r="G25" s="21">
+        <f>ABS(C25-E25)/E25</f>
         <v>3.0973451327433628E-2</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="8">
+      <c r="H25" s="21"/>
+      <c r="I25" s="8">
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="21" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C26" s="19">
         <v>381</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19">
         <v>326</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="11">
-        <f>ABS(C25-E25)/E25</f>
+      <c r="F26" s="19"/>
+      <c r="G26" s="21">
+        <f>ABS(C26-E26)/E26</f>
         <v>0.16871165644171779</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="8">
+      <c r="H26" s="21"/>
+      <c r="I26" s="8">
         <v>392</v>
       </c>
     </row>
@@ -3436,25 +3895,26 @@
       <c r="D41" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A17:C17"/>
-    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.15748031496062992" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>